<commit_message>
create CardsBaseJapan; move Images path
</commit_message>
<xml_diff>
--- a/CARD.xlsx
+++ b/CARD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwieb\Documents\MyMod\QuartermasterGeneral-v2-Chinese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C65E5B8-1863-4147-9AD7-92319CA41E9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389E7143-5FB0-401C-B79D-790F7884670D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-405" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24360" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -117,88 +117,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>77.潜艇支援太平洋诸岛
-　每有一个在东太平洋或邻接东太平洋的日本海军，你获得2分，美国需弃置其摸牌堆顶的2张牌。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>76.印度洋警备队
-　每有一个在孟加拉湾或邻接孟加拉湾的日本海军，你获得2分。英国需弃置其摸牌堆顶的2张牌。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>105.商船安全运输
 　在你的得分阶段，若在夏威夷没有同盟国的陆军，你获得1分。</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>103.大东亚共荣圈
-　在你的得分阶段，每有一个在印度尼西亚，新几内亚，东南亚的日本陆军，你获得1分。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>104.帝国的意图
 　在你的得分阶段，若在硫磺岛或菲律宾有日本陆军，你获得1分。</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>102.前进基地
-　在你的得分阶段，若在夏威夷或太平洋西北部或新西兰有日本陆军，你获得2分。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>97.丘克群岛
-　在你回合的任意时机使用。在太平洋中部或邻接太平洋中部的日本部队，在此回合中处于获得补给状态。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>96.奇袭
-　当你发动海战时使用。发动一次海战，再发动一次陆战。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>95.特种陆战队
-　当你设立海军时使用。在你设立海军的邻接地区，你可设立一至两个陆军。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>94.机动部队
-　在你的回合开始时使用。在北太平洋或邻接北太平洋的地区召集一个海军。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>93.关东军
-　在中国东部或四川或东北或蒙古处于补给状态的日本陆军将被移除时使用。本回合这个陆军不会被移除。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>92.神风特攻队
 　当同盟国邻接日本部队设立海军时使用。立刻移除其设立的海军。</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>91.攻陷新加坡
-　当你在东南亚发动陆战时使用。在南海发动海战，在东南亚召集陆军。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>90.驱逐舰运输
-　当你发动海战时使用。邻接战斗地区设立一至两个陆军。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>89.侵略中国
-　当你在中国东部或邻接中国东部的地区发动陆战时使用。在陆战地区设立陆军。在中国东部或邻接中国东部的地区发动陆战。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>88.战舰修理
 　当你处于补给状态的海军将被移除时使用。本回合这个海军不会被移除。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>87.万岁冲锋
-　当你发动陆战时使用。在战斗的地区或邻接地区发动陆战。</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1616,6 +1551,71 @@
 当同盟国获得制空权将意大利空军移除时使用。移除为获得制空权而使用的空军。
 </t>
     </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>76.印度洋警备队
+　每有一个位于或邻接&lt;孟加拉湾&gt;的日本海军，你获得 2 分。英国需弃置其摸牌堆顶的 2 张牌。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>77.潜艇支援太平洋诸岛
+　每有一个位于或邻接&lt;东太平洋&gt;的日本海军，你获得 2 分，美国需弃置其摸牌堆顶的 2 张牌。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>87.万岁冲锋
+　当你发动陆战时触发：在战斗的地区或邻接地区发动陆战。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>89.侵略中国
+　当你在&lt;中国东部&gt;或与之邻接的地区发动陆战时触发：在陆战地区设立陆军；在&lt;中国东部&gt;或与之邻接的地区发动陆战。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>90.驱逐舰运输
+　当你发动海战时触发：在与战斗海域相邻的地区设立一至两个陆军。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>91.攻陷新加坡
+　当你在&lt;东南亚&gt;发动陆战时触发：在南海发动海战，在东南亚征召陆军。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>93.关东军
+　在位于&lt;中国东部&gt;&lt;中国西部&gt;&lt;海参威&gt;&lt;蒙古地区&gt;且处于补给状态的日本陆军将被移除时触发：本回合此陆军不会被移除。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>94.机动部队
+　在你的回合开始时触发：在&lt;北太平洋&gt;或与之邻接的海域征召一支海军。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>95.特种陆战队
+　当你建设海军时触发：在与该海域相邻的一至两个地区设立陆军。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>96.奇袭
+　当你发动海战时触发：发动一次海战，再发动一次陆战。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>97.丘克群岛
+　在你回合的任意时机触发：位于或邻接&lt;中太平洋&gt;的日本部队在此回合中处于补给状态。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>102.前进基地
+　在你的计分阶段发动：若有位于&lt;夏威夷&gt;&lt;太平洋西北地区&gt;&lt;新西兰&gt;的日本陆军，你获得2分。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>103.大东亚共荣圈
+　在你的计分阶段发动：每有一个位于&lt;印度尼西亚&gt;&lt;新几内亚&gt;&lt;东南亚&gt;的日本陆军，获得 1 VP。</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1690,7 +1690,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1705,7 +1705,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1737,7 +1749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1758,6 +1770,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2042,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="100.5" customHeight="1"/>
@@ -2056,217 +2074,217 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>69</v>
+      <c r="B1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B2" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>67</v>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B3" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>64</v>
+      <c r="B3" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>61</v>
+      <c r="B4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>58</v>
+      <c r="B5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>55</v>
+      <c r="B6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>51</v>
+      <c r="B7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>53</v>
+      <c r="B8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="100.5" customHeight="1">
       <c r="B9" s="5" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="100.5" customHeight="1">
       <c r="B10" s="5" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="100.5" customHeight="1">
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="100.5" customHeight="1">
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>40</v>
+      <c r="B13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="B14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="100.5" customHeight="1">
+      <c r="B15" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="100.5" customHeight="1">
+      <c r="B16" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="100.5" customHeight="1">
+      <c r="B17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="100.5" customHeight="1">
+      <c r="B18" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="100.5" customHeight="1">
+      <c r="B19" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B15" s="2" t="s">
+    <row r="20" spans="2:4" ht="100.5" customHeight="1">
+      <c r="B20" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="100.5" customHeight="1">
-      <c r="B20" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>16</v>
@@ -2332,164 +2350,164 @@
     </row>
     <row r="26" spans="2:4" ht="100.5" customHeight="1">
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="100.5" customHeight="1">
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="100.5" customHeight="1">
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="100.5" customHeight="1">
       <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="100.5" customHeight="1">
       <c r="B30" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="100.5" customHeight="1">
       <c r="B31" s="2" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="100.5" customHeight="1">
       <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="100.5" customHeight="1">
       <c r="B33" s="2" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="100.5" customHeight="1">
       <c r="B34" s="2" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="100.5" customHeight="1">
       <c r="B35" s="2" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="100.5" customHeight="1">
       <c r="B36" s="2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="100.5" customHeight="1">
       <c r="B37" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="100.5" customHeight="1">
       <c r="B38" s="2" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="100.5" customHeight="1">
       <c r="B39" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="100.5" customHeight="1">
       <c r="B40" s="2" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D40" s="4"/>
     </row>
@@ -2519,486 +2537,486 @@
   <sheetData>
     <row r="1" spans="2:4" ht="100.5" customHeight="1">
       <c r="B1" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="100.5" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="100.5" customHeight="1">
       <c r="B3" s="2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="100.5" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="100.5" customHeight="1">
       <c r="B5" s="2" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="100.5" customHeight="1">
       <c r="B6" s="2" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="100.5" customHeight="1">
       <c r="B7" s="2" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="100.5" customHeight="1">
       <c r="B8" s="2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="100.5" customHeight="1">
       <c r="B9" s="2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="100.5" customHeight="1">
       <c r="B10" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="100.5" customHeight="1">
       <c r="B11" s="2" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="100.5" customHeight="1">
       <c r="B12" s="2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="100.5" customHeight="1">
       <c r="B13" s="2" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="100.5" customHeight="1">
       <c r="B14" s="2" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="100.5" customHeight="1">
       <c r="B15" s="2" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="100.5" customHeight="1">
       <c r="B16" s="2" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="100.5" customHeight="1">
       <c r="B17" s="2" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="100.5" customHeight="1">
       <c r="B18" s="2" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="100.5" customHeight="1">
       <c r="B19" s="6" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="100.5" customHeight="1">
       <c r="B20" s="2" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="100.5" customHeight="1">
       <c r="B21" s="2" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="100.5" customHeight="1">
       <c r="B22" s="2" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="100.5" customHeight="1">
       <c r="B23" s="2" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="100.5" customHeight="1">
       <c r="B24" s="2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="100.5" customHeight="1">
       <c r="B25" s="2" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="100.5" customHeight="1">
       <c r="B26" s="2" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="100.5" customHeight="1">
       <c r="B27" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="100.5" customHeight="1">
       <c r="B28" s="2" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="100.5" customHeight="1">
       <c r="B29" s="2" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="100.5" customHeight="1">
       <c r="B30" s="6" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="100.5" customHeight="1">
       <c r="B31" s="2" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="100.5" customHeight="1">
       <c r="B32" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="100.5" customHeight="1">
       <c r="B33" s="2" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="100.5" customHeight="1">
       <c r="B34" s="2" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="100.5" customHeight="1">
       <c r="B35" s="2" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="100.5" customHeight="1">
       <c r="B36" s="2" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="100.5" customHeight="1">
       <c r="B37" s="2" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="100.5" customHeight="1">
       <c r="B38" s="6" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="100.5" customHeight="1">
       <c r="B39" s="6" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="100.5" customHeight="1">
       <c r="B40" s="6" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="100.5" customHeight="1">
       <c r="B41" s="6" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="100.5" customHeight="1">
       <c r="B42" s="6" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="100.5" customHeight="1">
       <c r="B43" s="6" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="100.5" customHeight="1">
       <c r="B44" s="6" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="100.5" customHeight="1">

</xml_diff>